<commit_message>
1870 gereed, 1890 toegevoegd
</commit_message>
<xml_diff>
--- a/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.2.xlsx
+++ b/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\0.98-3-Validatie-_en_conformiteitsregels_TPOD\documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96358E1-2CBA-463F-89CF-62B5C96FA3D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA7DB6C-23A3-406B-BFC8-9D1C2C9F71ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TotaalOverzicht" sheetId="6" r:id="rId1"/>
@@ -2182,12 +2182,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -2244,7 +2250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2311,6 +2317,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -20878,8 +20891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFBB57E-3244-4327-8FA7-3800EF9A5F79}">
   <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20952,7 +20965,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="31" t="s">
         <v>197</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -21000,7 +21013,7 @@
       <c r="P2" s="14"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="31" t="s">
         <v>198</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -21288,7 +21301,7 @@
       <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="31" t="s">
         <v>532</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -21336,7 +21349,7 @@
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="31" t="s">
         <v>533</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -21384,7 +21397,7 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="31" t="s">
         <v>534</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -21432,7 +21445,7 @@
       <c r="P11" s="14"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -21480,7 +21493,7 @@
       <c r="P12" s="14"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="33" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -21528,7 +21541,7 @@
       <c r="P13" s="14"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="33" t="s">
         <v>186</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -21576,7 +21589,7 @@
       <c r="P14" s="14"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -21624,7 +21637,7 @@
       <c r="P15" s="14"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -21672,7 +21685,7 @@
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -21720,7 +21733,7 @@
       <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="33" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -21768,7 +21781,7 @@
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -21816,7 +21829,7 @@
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -21912,7 +21925,7 @@
       <c r="P21" s="14"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -25871,7 +25884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B00849-1664-4F48-9EE1-9C727831D253}">
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>

</xml_diff>